<commit_message>
Fits of H2 resistance drops
</commit_message>
<xml_diff>
--- a/Measurements/1024_1258_wo3189_r13 RT1/data/H2 drop fit/1024_1258_wo3189_r13_resistance_fit_coef.xlsx
+++ b/Measurements/1024_1258_wo3189_r13 RT1/data/H2 drop fit/1024_1258_wo3189_r13_resistance_fit_coef.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rijk\Documents\MEP\MEP_control_software\1024_1258_wo3189_r13 RT1\data\H2 drop fit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{86AF6D20-D586-443F-8492-008F76B52A96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C20A164-9EF3-412B-8E1E-B849F4FD1D14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1024_1258_wo3189_r13_resistance" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -855,16 +863,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1">
         <v>13845.300071609699</v>
       </c>
@@ -876,7 +884,7 @@
         <v>138453000716.09698</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>760.24230772141505</v>
       </c>
@@ -887,8 +895,12 @@
         <f>B2*A2</f>
         <v>7.6024230772141514E-3</v>
       </c>
+      <c r="D2" s="1">
+        <f>C2^-1</f>
+        <v>131.53700995636279</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>0.70629454319895801</v>
       </c>

</xml_diff>